<commit_message>
begin adding log file export
</commit_message>
<xml_diff>
--- a/FinalProject/mock_course_list.xlsx
+++ b/FinalProject/mock_course_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/administrator/Documents/Projects/CS232_Assignments/FinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E609CC-B7BC-C645-A545-E718B706FC6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084CC0F0-1657-C045-8AED-793CA3A961FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23960" yWindow="1040" windowWidth="10000" windowHeight="16940" xr2:uid="{39020F34-3ED9-314B-B943-F01ABA66F3DB}"/>
+    <workbookView xWindow="15120" yWindow="460" windowWidth="10000" windowHeight="16940" xr2:uid="{39020F34-3ED9-314B-B943-F01ABA66F3DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,14 +516,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B8756F-2FB0-0641-BBB1-567417D35217}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>